<commit_message>
created a model ProdecureItem to load the ul-in UserEngagement-detailsPage
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/11_businessModels/dataModel_userIntegration.xlsx
+++ b/02_work_doc/01_daten/11_businessModels/dataModel_userIntegration.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="German" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="English" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="German" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="English" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -113,12 +113,17 @@
     <t xml:space="preserve">Tem restota turibus sunt pel modignati aut eniae volor rem idelibus idic tescit, quunt fuga. Nam ut res et dem quiam resci aut eum re plati nus rerores atquo temporit aciaspe ritempo rpossit et plaborum invel et quideni denis. Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit imoluptatus anditi vent, utecus dolesci officil loriae nos quae. Nequatia nest ea sa es net omnis voluptinciti occabo. Tem restota turibus sunt pel modignati aut eniae volor rem idelibus idic tescit, quunt fuga. Nam ut res et dem quiam resci aut eum re plati nus rerores atquo temporit aciaspe ritempo rpossit et plaborum invel et quideni denis. Et fugit od eos eatum expedit, imint as quas comniminus electibustis.</t>
   </si>
   <si>
-    <t xml:space="preserve">Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiure.
-Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam.
-Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit  </t>
+    <t xml:space="preserve">Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiure;
+Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam;
+Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit; </t>
   </si>
   <si>
     <t xml:space="preserve">Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiures es doluptatur santius ulparciis et ad eum aceptiistion cum quianihictem unt ut pel ma dolorpo rruntur, accat. Ent, que nimi, quas si odi optatis ex estisque ommossi tatur, vendit por sum ellecatur repudanda simusae et enis ne nus. Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit imoluptatus anditi vent, utecus dolesci officil loriae nos quae. Nequatia nest ea sa es net omnis voluptinciti occabo. Tem restota turibus sunt pel modignati aut eniae volor rem idelibus idic tescit, quunt fuga. Nam ut res et dem quiam resci aut eum re plati nus rerores atquo temporit aciaspe ritempo rpossit et plaborum invel et quideni denis. Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit imoluptatus anditi vent, utecus dolesci officil loriae nos quae. Nequatia nest ea sa es net omnis voluptinciti occabo. Tem restota turibus sunt pel modignati aut eniae volor rem idelibus idic tescit, quunt fuga. Nam ut res et dem quiam resci aut eum re plati nus rerores atquo temporit aciaspe ritempo rpossit et plaborum invel et quideni denis. Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiure;
+Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam;
+Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit;</t>
   </si>
   <si>
     <t xml:space="preserve">Methoden für die Konzeptionsphase</t>
@@ -227,7 +232,7 @@
   <fonts count="4">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -311,194 +316,22 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="163.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -554,7 +387,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="409.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="710.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
@@ -604,7 +437,7 @@
         <v>31</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +445,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -623,7 +456,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -641,7 +474,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -651,59 +484,59 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -711,49 +544,49 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed data_import script so that only procedureItems which are not only whitespaces are imported
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/11_businessModels/dataModel_userIntegration.xlsx
+++ b/02_work_doc/01_daten/11_businessModels/dataModel_userIntegration.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t xml:space="preserve">Konkreter_Ablauf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beobachtungen der Teilnehmenden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personas</t>
   </si>
   <si>
     <t xml:space="preserve">Methoden für die Analysephase</t>
@@ -124,6 +130,9 @@
     <t xml:space="preserve">Con rest voles molor se reptur, erum sum autaquiae prae nonsequat quas ex exero dolupti dolupta tempossimi, volestiure;
 Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam;
 Et fugit od eos eatum expedit, imint as quas comniminus electibustis doloribus. Ent que volore doles eos es dolupta voluptibusam cus sam que nimodios as dolori dolor aut dolorem rem que voluptasimus eum imenihit;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teilnehmende Beobachtungen</t>
   </si>
   <si>
     <t xml:space="preserve">Methoden für die Konzeptionsphase</t>
@@ -321,10 +330,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R7" activeCellId="0" sqref="R7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -386,58 +395,70 @@
       <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="710.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,9 +466,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -456,9 +483,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -491,52 +524,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,49 +577,49 @@
         <v>0</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>